<commit_message>
Добавлены анимации:  upward_attack_from_the_spot  downward_attack_from_the_spot  attack_in_motion Дорабатаны анимации:  attack_from_the_spot
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Дроид штурмовик</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>walk_blaster_stop</t>
+  </si>
+  <si>
+    <t>upward_attack_from_the_spot</t>
+  </si>
+  <si>
+    <t>downward_attack_from_the_spot</t>
+  </si>
+  <si>
+    <t>attack_in_motion</t>
   </si>
 </sst>
 </file>
@@ -557,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -617,6 +626,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -914,14 +925,14 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1009,22 +1020,28 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="37"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="21" t="s">

</xml_diff>

<commit_message>
Добавлены анимации:  death_from_a_lightsword_body  death_from_a_lightsword_legs  death_from_a_lightsword_head  death_from_a_pressing_upward  death_from_a_pressing_downward  death_from_a_blaster_head  death_from_a_blaster_closure
Переименованы анимации:
 из upward_attack_from_the_spot в attack_from_the_spot_upward
 из downward_attack_from_the_spot в attack_from_the_spot_downward
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Дроид штурмовик</t>
   </si>
@@ -141,13 +141,40 @@
     <t>walk_blaster_stop</t>
   </si>
   <si>
-    <t>upward_attack_from_the_spot</t>
-  </si>
-  <si>
-    <t>downward_attack_from_the_spot</t>
-  </si>
-  <si>
     <t>attack_in_motion</t>
+  </si>
+  <si>
+    <t>death_from_a_lightsword_head</t>
+  </si>
+  <si>
+    <t>death_from_a_lightsword_body</t>
+  </si>
+  <si>
+    <t>death_from_a_lightsword_legs</t>
+  </si>
+  <si>
+    <t>death_from_a_pressing_upward</t>
+  </si>
+  <si>
+    <t>death_from_a_pressing_downward</t>
+  </si>
+  <si>
+    <t>death_from_a_push_upward</t>
+  </si>
+  <si>
+    <t>death_from_a_push_downward</t>
+  </si>
+  <si>
+    <t>death_from_a_blaster_head</t>
+  </si>
+  <si>
+    <t>death_from_a_blaster_closure</t>
+  </si>
+  <si>
+    <t>attack_from_the_spot_upward</t>
+  </si>
+  <si>
+    <t>attack_from_the_spot_downward</t>
   </si>
 </sst>
 </file>
@@ -924,14 +951,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1021,7 +1048,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -1030,7 +1057,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -1039,7 +1066,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="37"/>
     </row>
@@ -1061,21 +1088,27 @@
       <c r="A15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="20"/>
+      <c r="B17" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
@@ -1089,14 +1122,18 @@
       <c r="A19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="24"/>
+      <c r="B19" s="24" t="s">
+        <v>45</v>
+      </c>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="20" t="s">
+        <v>46</v>
+      </c>
       <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1">
@@ -1110,14 +1147,18 @@
       <c r="A22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="24"/>
+      <c r="B22" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1">
@@ -1131,14 +1172,18 @@
       <c r="A25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="24"/>
+      <c r="B25" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1">
       <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="20"/>
+      <c r="B26" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1">

</xml_diff>